<commit_message>
slight adjustments to 7 statuses of countries
</commit_message>
<xml_diff>
--- a/AbsMaster.xlsx
+++ b/AbsMaster.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ciaraweets/Dropbox/R Projects/ABS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44759020-3EB4-1D48-A91B-D32795E2B0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66682D73-86A6-2D42-A084-B40180072EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33000" yWindow="3820" windowWidth="26440" windowHeight="14940"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AbsMaster" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6435" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6435" uniqueCount="425">
   <si>
     <t>Country</t>
   </si>
@@ -1289,12 +1289,18 @@
   </si>
   <si>
     <t>Justification</t>
+  </si>
+  <si>
+    <t>Access is restricted but benefit-sharing is not mandated</t>
+  </si>
+  <si>
+    <t>Fines, criminalization, and access restrictions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2128,11 +2134,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1609"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A1252" zoomScale="179" workbookViewId="0">
+      <selection activeCell="C1267" sqref="C1267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8927,7 +8933,7 @@
         <v>11</v>
       </c>
       <c r="C485" t="s">
-        <v>40</v>
+        <v>153</v>
       </c>
       <c r="D485" t="s">
         <v>7</v>
@@ -8941,7 +8947,7 @@
         <v>14</v>
       </c>
       <c r="C486" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D486" t="s">
         <v>7</v>
@@ -8955,7 +8961,7 @@
         <v>17</v>
       </c>
       <c r="C487" t="s">
-        <v>40</v>
+        <v>423</v>
       </c>
       <c r="D487" t="s">
         <v>7</v>
@@ -8969,7 +8975,7 @@
         <v>20</v>
       </c>
       <c r="C488" t="s">
-        <v>40</v>
+        <v>167</v>
       </c>
       <c r="D488" t="s">
         <v>7</v>
@@ -8983,7 +8989,7 @@
         <v>23</v>
       </c>
       <c r="C489" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D489" t="s">
         <v>7</v>
@@ -10677,7 +10683,7 @@
         <v>2</v>
       </c>
       <c r="C610" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D610" t="s">
         <v>27</v>
@@ -10691,7 +10697,7 @@
         <v>5</v>
       </c>
       <c r="C611" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D611" t="s">
         <v>7</v>
@@ -10705,7 +10711,7 @@
         <v>8</v>
       </c>
       <c r="C612" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D612" t="s">
         <v>10</v>
@@ -12620,7 +12626,7 @@
         <v>11</v>
       </c>
       <c r="C749" t="s">
-        <v>40</v>
+        <v>153</v>
       </c>
       <c r="D749" t="s">
         <v>7</v>
@@ -13978,7 +13984,7 @@
         <v>14</v>
       </c>
       <c r="C846" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D846" t="s">
         <v>7</v>
@@ -13992,7 +13998,7 @@
         <v>17</v>
       </c>
       <c r="C847" t="s">
-        <v>57</v>
+        <v>423</v>
       </c>
       <c r="D847" t="s">
         <v>275</v>
@@ -15980,7 +15986,7 @@
         <v>11</v>
       </c>
       <c r="C989" t="s">
-        <v>40</v>
+        <v>153</v>
       </c>
       <c r="D989" t="s">
         <v>7</v>
@@ -16638,7 +16644,7 @@
         <v>8</v>
       </c>
       <c r="C1036" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D1036" t="s">
         <v>317</v>
@@ -16652,7 +16658,7 @@
         <v>11</v>
       </c>
       <c r="C1037" t="s">
-        <v>153</v>
+        <v>40</v>
       </c>
       <c r="D1037" t="s">
         <v>317</v>
@@ -16666,7 +16672,7 @@
         <v>14</v>
       </c>
       <c r="C1038" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D1038" t="s">
         <v>317</v>
@@ -16680,7 +16686,7 @@
         <v>17</v>
       </c>
       <c r="C1039" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D1039" t="s">
         <v>317</v>
@@ -16694,7 +16700,7 @@
         <v>20</v>
       </c>
       <c r="C1040" t="s">
-        <v>167</v>
+        <v>40</v>
       </c>
       <c r="D1040" t="s">
         <v>317</v>
@@ -16708,7 +16714,7 @@
         <v>23</v>
       </c>
       <c r="C1041" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="D1041" t="s">
         <v>317</v>
@@ -19788,7 +19794,7 @@
         <v>11</v>
       </c>
       <c r="C1261" t="s">
-        <v>40</v>
+        <v>153</v>
       </c>
       <c r="D1261" t="s">
         <v>7</v>
@@ -19802,7 +19808,7 @@
         <v>14</v>
       </c>
       <c r="C1262" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D1262" t="s">
         <v>7</v>
@@ -19816,7 +19822,7 @@
         <v>17</v>
       </c>
       <c r="C1263" t="s">
-        <v>40</v>
+        <v>423</v>
       </c>
       <c r="D1263" t="s">
         <v>7</v>
@@ -19830,7 +19836,7 @@
         <v>20</v>
       </c>
       <c r="C1264" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D1264" t="s">
         <v>22</v>
@@ -19844,7 +19850,7 @@
         <v>23</v>
       </c>
       <c r="C1265" t="s">
-        <v>40</v>
+        <v>424</v>
       </c>
       <c r="D1265" t="s">
         <v>76</v>

</xml_diff>